<commit_message>
Updated output to reflect the previous commit.
Rewrote the output table docs/ic_maps_stats.xlsx to
reflect the change in 09b994b0e1d04b5664c1a0b2baef76788f64da5f.
</commit_message>
<xml_diff>
--- a/docs/ic_maps_stats.xlsx
+++ b/docs/ic_maps_stats.xlsx
@@ -693,7 +693,7 @@
         <v>-0.1884615384615385</v>
       </c>
       <c r="L2">
-        <v>-0.1884615384615385</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0.7981974413354439</v>
@@ -746,7 +746,7 @@
         <v>0.03571428571428571</v>
       </c>
       <c r="L3">
-        <v>0.03571428571428571</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0.2672612419124245</v>
@@ -799,7 +799,7 @@
         <v>0.08653846153846154</v>
       </c>
       <c r="L4">
-        <v>0.08653846153846154</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0.6240377207533832</v>
@@ -852,7 +852,7 @@
         <v>-0.04464285714285714</v>
       </c>
       <c r="L5">
-        <v>-0.04464285714285714</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0.3340765523905307</v>
@@ -926,7 +926,7 @@
         <v>-12.07692307692308</v>
       </c>
       <c r="L6">
-        <v>-12.07692307692308</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>68.00576277595204</v>
@@ -1000,7 +1000,7 @@
         <v>-2.535714285714286</v>
       </c>
       <c r="L7">
-        <v>-2.535714285714286</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>11.54438751588335</v>
@@ -1074,7 +1074,7 @@
         <v>0.3634615384615384</v>
       </c>
       <c r="L8">
-        <v>0.3634615384615384</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>2.223848355507998</v>
@@ -1148,7 +1148,7 @@
         <v>-0.1821428571428571</v>
       </c>
       <c r="L9">
-        <v>-0.1821428571428571</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>1.435283582097615</v>
@@ -1222,7 +1222,7 @@
         <v>0.1346153846153846</v>
       </c>
       <c r="L10">
-        <v>0.1346153846153846</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0.9707253433941503</v>
@@ -1275,7 +1275,7 @@
         <v>-0.01071428571428571</v>
       </c>
       <c r="L11">
-        <v>-0.01071428571428571</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0.08017837257372723</v>
@@ -1349,7 +1349,7 @@
         <v>8.419230769230769</v>
       </c>
       <c r="L12">
-        <v>8.419230769230769</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>55.23926224628936</v>
@@ -1423,7 +1423,7 @@
         <v>6.889285714285714</v>
       </c>
       <c r="L13">
-        <v>6.889285714285714</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>45.79617164853781</v>
@@ -1497,7 +1497,7 @@
         <v>-38.50961538461537</v>
       </c>
       <c r="L14">
-        <v>-38.50961538461537</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>103.2469840220677</v>
@@ -1571,7 +1571,7 @@
         <v>6.175</v>
       </c>
       <c r="L15">
-        <v>6.175</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>40.49271651678968</v>
@@ -1645,7 +1645,7 @@
         <v>-1.723076923076922</v>
       </c>
       <c r="L16">
-        <v>-1.723076923076922</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <v>60.20277048990882</v>
@@ -1719,7 +1719,7 @@
         <v>-1.101785714285715</v>
       </c>
       <c r="L17">
-        <v>-1.101785714285715</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <v>47.1754038035285</v>
@@ -1793,7 +1793,7 @@
         <v>-2.646153846153846</v>
       </c>
       <c r="L18">
-        <v>-2.646153846153846</v>
+        <v>0</v>
       </c>
       <c r="M18">
         <v>23.03032494929208</v>
@@ -1867,7 +1867,7 @@
         <v>1.666071428571429</v>
       </c>
       <c r="L19">
-        <v>1.666071428571429</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <v>20.84401180008488</v>
@@ -1941,7 +1941,7 @@
         <v>-14.49230769230769</v>
       </c>
       <c r="L20">
-        <v>-14.49230769230769</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>45.1071484537535</v>
@@ -2015,7 +2015,7 @@
         <v>0.8071428571428576</v>
       </c>
       <c r="L21">
-        <v>0.8071428571428576</v>
+        <v>0</v>
       </c>
       <c r="M21">
         <v>13.71808172572851</v>
@@ -2089,7 +2089,7 @@
         <v>-1.430769230769231</v>
       </c>
       <c r="L22">
-        <v>-1.430769230769231</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>25.04142871998038</v>
@@ -2163,7 +2163,7 @@
         <v>8.392857142857142</v>
       </c>
       <c r="L23">
-        <v>8.392857142857142</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <v>25.35272520508741</v>
@@ -2237,7 +2237,7 @@
         <v>-0.7384615384615386</v>
       </c>
       <c r="L24">
-        <v>-0.7384615384615386</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <v>5.529569491669096</v>
@@ -2311,7 +2311,7 @@
         <v>0.4714285714285714</v>
       </c>
       <c r="L25">
-        <v>0.4714285714285714</v>
+        <v>0</v>
       </c>
       <c r="M25">
         <v>5.251898852647636</v>
@@ -2385,7 +2385,7 @@
         <v>-2.578846153846154</v>
       </c>
       <c r="L26">
-        <v>-2.578846153846154</v>
+        <v>0</v>
       </c>
       <c r="M26">
         <v>23.34127318585367</v>
@@ -2459,7 +2459,7 @@
         <v>5.75</v>
       </c>
       <c r="L27">
-        <v>5.75</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <v>24.55229668946009</v>
@@ -2533,7 +2533,7 @@
         <v>13.07692307692308</v>
       </c>
       <c r="L28">
-        <v>13.07692307692308</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <v>53.68964779678652</v>
@@ -2607,7 +2607,7 @@
         <v>-0.1071428571428571</v>
       </c>
       <c r="L29">
-        <v>-0.1071428571428571</v>
+        <v>0</v>
       </c>
       <c r="M29">
         <v>22.32338241838372</v>
@@ -2681,7 +2681,7 @@
         <v>-0.8519230769230768</v>
       </c>
       <c r="L30">
-        <v>-0.8519230769230768</v>
+        <v>0</v>
       </c>
       <c r="M30">
         <v>111.1598169222586</v>
@@ -2755,7 +2755,7 @@
         <v>-13.53392857142857</v>
       </c>
       <c r="L31">
-        <v>-13.53392857142857</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <v>94.60562788715093</v>
@@ -2829,7 +2829,7 @@
         <v>-35.82692307692308</v>
       </c>
       <c r="L32">
-        <v>-35.82692307692308</v>
+        <v>0</v>
       </c>
       <c r="M32">
         <v>106.4930912154465</v>
@@ -2903,7 +2903,7 @@
         <v>-17.17321428571428</v>
       </c>
       <c r="L33">
-        <v>-17.17321428571428</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>91.74817212164142</v>
@@ -2977,7 +2977,7 @@
         <v>-34.48076923076923</v>
       </c>
       <c r="L34">
-        <v>-34.48076923076923</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>128.027765123562</v>
@@ -3051,7 +3051,7 @@
         <v>-16.09285714285715</v>
       </c>
       <c r="L35">
-        <v>-16.09285714285715</v>
+        <v>0</v>
       </c>
       <c r="M35">
         <v>54.39874282351776</v>
@@ -3125,7 +3125,7 @@
         <v>0.8480769230769228</v>
       </c>
       <c r="L36">
-        <v>0.8480769230769228</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>18.66874803225984</v>
@@ -3199,7 +3199,7 @@
         <v>-3.455357142857143</v>
       </c>
       <c r="L37">
-        <v>-3.455357142857143</v>
+        <v>0</v>
       </c>
       <c r="M37">
         <v>16.67586082982177</v>
@@ -3273,7 +3273,7 @@
         <v>-3.863461538461539</v>
       </c>
       <c r="L38">
-        <v>-3.863461538461539</v>
+        <v>0</v>
       </c>
       <c r="M38">
         <v>23.9415794591437</v>
@@ -3347,7 +3347,7 @@
         <v>-1.403571428571428</v>
       </c>
       <c r="L39">
-        <v>-1.403571428571428</v>
+        <v>0</v>
       </c>
       <c r="M39">
         <v>21.28791346610229</v>
@@ -3527,7 +3527,7 @@
         <v>0.5980769230769231</v>
       </c>
       <c r="L42">
-        <v>0.5980769230769231</v>
+        <v>0</v>
       </c>
       <c r="M42">
         <v>3.819171986260045</v>
@@ -3601,7 +3601,7 @@
         <v>-0.1946428571428571</v>
       </c>
       <c r="L43">
-        <v>-0.1946428571428571</v>
+        <v>0</v>
       </c>
       <c r="M43">
         <v>2.83974516416572</v>
@@ -3781,7 +3781,7 @@
         <v>-0.2711538461538462</v>
       </c>
       <c r="L46">
-        <v>-0.2711538461538462</v>
+        <v>0</v>
       </c>
       <c r="M46">
         <v>1.16000955683378</v>
@@ -3834,7 +3834,7 @@
         <v>0.05</v>
       </c>
       <c r="L47">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>0.3741657386773943</v>
@@ -3887,7 +3887,7 @@
         <v>0.1557692307692308</v>
       </c>
       <c r="L48">
-        <v>0.1557692307692308</v>
+        <v>0</v>
       </c>
       <c r="M48">
         <v>1.123267897356089</v>
@@ -3940,7 +3940,7 @@
         <v>-0.07857142857142858</v>
       </c>
       <c r="L49">
-        <v>-0.07857142857142858</v>
+        <v>0</v>
       </c>
       <c r="M49">
         <v>0.5879747322073333</v>
@@ -4014,7 +4014,7 @@
         <v>-22.80576923076923</v>
       </c>
       <c r="L50">
-        <v>-22.80576923076923</v>
+        <v>0</v>
       </c>
       <c r="M50">
         <v>126.7429178335631</v>
@@ -4088,7 +4088,7 @@
         <v>-4.903571428571429</v>
       </c>
       <c r="L51">
-        <v>-4.903571428571429</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <v>17.0868792223285</v>
@@ -4162,7 +4162,7 @@
         <v>0.8499999999999999</v>
       </c>
       <c r="L52">
-        <v>0.8499999999999999</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>4.516961498227611</v>
@@ -4236,7 +4236,7 @@
         <v>-0.4125</v>
       </c>
       <c r="L53">
-        <v>-0.4125</v>
+        <v>0</v>
       </c>
       <c r="M53">
         <v>1.923922366606114</v>
@@ -4310,7 +4310,7 @@
         <v>0.2461538461538462</v>
       </c>
       <c r="L54">
-        <v>0.2461538461538462</v>
+        <v>0</v>
       </c>
       <c r="M54">
         <v>1.775040627920733</v>
@@ -4363,7 +4363,7 @@
         <v>0.01428571428571429</v>
       </c>
       <c r="L55">
-        <v>0.01428571428571429</v>
+        <v>0</v>
       </c>
       <c r="M55">
         <v>0.1069044967649698</v>
@@ -4437,7 +4437,7 @@
         <v>8.00576923076923</v>
       </c>
       <c r="L56">
-        <v>8.00576923076923</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>64.72322192427866</v>
@@ -4511,7 +4511,7 @@
         <v>7.655357142857142</v>
       </c>
       <c r="L57">
-        <v>7.655357142857142</v>
+        <v>0</v>
       </c>
       <c r="M57">
         <v>45.08029571429529</v>
@@ -4585,7 +4585,7 @@
         <v>-45.32884615384614</v>
       </c>
       <c r="L58">
-        <v>-45.32884615384614</v>
+        <v>0</v>
       </c>
       <c r="M58">
         <v>104.2723100433657</v>
@@ -4659,7 +4659,7 @@
         <v>4.316071428571428</v>
       </c>
       <c r="L59">
-        <v>4.316071428571428</v>
+        <v>0</v>
       </c>
       <c r="M59">
         <v>65.02525880354135</v>
@@ -4733,7 +4733,7 @@
         <v>-8.451923076923078</v>
       </c>
       <c r="L60">
-        <v>-8.451923076923078</v>
+        <v>0</v>
       </c>
       <c r="M60">
         <v>118.3145267967176</v>
@@ -4807,7 +4807,7 @@
         <v>1.1</v>
       </c>
       <c r="L61">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="M61">
         <v>80.38222327220009</v>
@@ -4881,7 +4881,7 @@
         <v>-0.5730769230769235</v>
       </c>
       <c r="L62">
-        <v>-0.5730769230769235</v>
+        <v>0</v>
       </c>
       <c r="M62">
         <v>47.94519385586337</v>
@@ -4955,7 +4955,7 @@
         <v>-0.737499999999999</v>
       </c>
       <c r="L63">
-        <v>-0.737499999999999</v>
+        <v>0</v>
       </c>
       <c r="M63">
         <v>37.88021101265983</v>
@@ -5029,7 +5029,7 @@
         <v>-20.57115384615385</v>
       </c>
       <c r="L64">
-        <v>-20.57115384615385</v>
+        <v>0</v>
       </c>
       <c r="M64">
         <v>81.76956703297499</v>
@@ -5103,7 +5103,7 @@
         <v>-2.578571428571428</v>
       </c>
       <c r="L65">
-        <v>-2.578571428571428</v>
+        <v>0</v>
       </c>
       <c r="M65">
         <v>37.89881127560461</v>
@@ -5177,7 +5177,7 @@
         <v>0.1442307692307696</v>
       </c>
       <c r="L66">
-        <v>0.1442307692307696</v>
+        <v>0</v>
       </c>
       <c r="M66">
         <v>46.43803973781406</v>
@@ -5251,7 +5251,7 @@
         <v>10.97142857142857</v>
       </c>
       <c r="L67">
-        <v>10.97142857142857</v>
+        <v>0</v>
       </c>
       <c r="M67">
         <v>34.94847487522017</v>
@@ -5325,7 +5325,7 @@
         <v>-0.5942307692307691</v>
       </c>
       <c r="L68">
-        <v>-0.5942307692307691</v>
+        <v>0</v>
       </c>
       <c r="M68">
         <v>10.13018036851479</v>
@@ -5399,7 +5399,7 @@
         <v>0.2982142857142857</v>
       </c>
       <c r="L69">
-        <v>0.2982142857142857</v>
+        <v>0</v>
       </c>
       <c r="M69">
         <v>8.284980738912786</v>
@@ -5473,7 +5473,7 @@
         <v>3.509615384615385</v>
       </c>
       <c r="L70">
-        <v>3.509615384615385</v>
+        <v>0</v>
       </c>
       <c r="M70">
         <v>29.73522542745757</v>
@@ -5547,7 +5547,7 @@
         <v>6.126785714285715</v>
       </c>
       <c r="L71">
-        <v>6.126785714285715</v>
+        <v>0</v>
       </c>
       <c r="M71">
         <v>34.52074733769891</v>
@@ -5621,7 +5621,7 @@
         <v>17.23653846153846</v>
       </c>
       <c r="L72">
-        <v>17.23653846153846</v>
+        <v>0</v>
       </c>
       <c r="M72">
         <v>70.46091679524149</v>
@@ -5695,7 +5695,7 @@
         <v>0.9160714285714281</v>
       </c>
       <c r="L73">
-        <v>0.9160714285714281</v>
+        <v>0</v>
       </c>
       <c r="M73">
         <v>24.1317955236407</v>
@@ -5769,7 +5769,7 @@
         <v>1.188461538461534</v>
       </c>
       <c r="L74">
-        <v>1.188461538461534</v>
+        <v>0</v>
       </c>
       <c r="M74">
         <v>273.4907007444041</v>
@@ -5843,7 +5843,7 @@
         <v>-33.1375</v>
       </c>
       <c r="L75">
-        <v>-33.1375</v>
+        <v>0</v>
       </c>
       <c r="M75">
         <v>237.5139686322775</v>
@@ -5917,7 +5917,7 @@
         <v>-38.43461538461538</v>
       </c>
       <c r="L76">
-        <v>-38.43461538461538</v>
+        <v>0</v>
       </c>
       <c r="M76">
         <v>118.4800287375602</v>
@@ -5991,7 +5991,7 @@
         <v>-11.93035714285714</v>
       </c>
       <c r="L77">
-        <v>-11.93035714285714</v>
+        <v>0</v>
       </c>
       <c r="M77">
         <v>54.1960847953324</v>
@@ -6065,7 +6065,7 @@
         <v>-27.47692307692308</v>
       </c>
       <c r="L78">
-        <v>-27.47692307692308</v>
+        <v>0</v>
       </c>
       <c r="M78">
         <v>177.8442958732741</v>
@@ -6139,7 +6139,7 @@
         <v>-18.84464285714285</v>
       </c>
       <c r="L79">
-        <v>-18.84464285714285</v>
+        <v>0</v>
       </c>
       <c r="M79">
         <v>92.66315717722955</v>
@@ -6213,7 +6213,7 @@
         <v>2.874999999999999</v>
       </c>
       <c r="L80">
-        <v>2.874999999999999</v>
+        <v>0</v>
       </c>
       <c r="M80">
         <v>30.30460312540383</v>
@@ -6287,7 +6287,7 @@
         <v>-6.9625</v>
       </c>
       <c r="L81">
-        <v>-6.9625</v>
+        <v>0</v>
       </c>
       <c r="M81">
         <v>30.03947440830605</v>
@@ -6361,7 +6361,7 @@
         <v>-9.107692307692307</v>
       </c>
       <c r="L82">
-        <v>-9.107692307692307</v>
+        <v>0</v>
       </c>
       <c r="M82">
         <v>33.94942516567755</v>
@@ -6435,7 +6435,7 @@
         <v>0.1267857142857146</v>
       </c>
       <c r="L83">
-        <v>0.1267857142857146</v>
+        <v>0</v>
       </c>
       <c r="M83">
         <v>25.15588845630332</v>
@@ -6615,7 +6615,7 @@
         <v>1.128846153846154</v>
       </c>
       <c r="L86">
-        <v>1.128846153846154</v>
+        <v>0</v>
       </c>
       <c r="M86">
         <v>6.288250373528472</v>
@@ -6689,7 +6689,7 @@
         <v>-0.4089285714285715</v>
       </c>
       <c r="L87">
-        <v>-0.4089285714285715</v>
+        <v>0</v>
       </c>
       <c r="M87">
         <v>4.63101311459301</v>

</xml_diff>